<commit_message>
tie break three teams
completed tie break with three team for eu uefa and wc fifa
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/uefa/eu/goals_eu_uefa_men.xlsx
+++ b/data/out/wiki/men/uefa/eu/goals_eu_uefa_men.xlsx
@@ -621,7 +621,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -692,7 +692,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -834,7 +834,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['France', 'Belgium']</t>
+          <t>['Belgium', 'France']</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1319,7 +1319,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['West Germany', 'Spain']</t>
+          <t>['Spain', 'West Germany']</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1386,7 +1386,7 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>['West Germany', 'Spain']</t>
+          <t>['Spain', 'West Germany']</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1453,7 +1453,7 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['West Germany', 'Spain']</t>
+          <t>['Spain', 'West Germany']</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1658,7 +1658,7 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1725,7 +1725,7 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1796,7 +1796,7 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2084,7 +2084,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>['West Germany', 'Italy']</t>
+          <t>['Italy', 'West Germany']</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -3129,7 +3129,7 @@
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3196,7 +3196,7 @@
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3271,7 +3271,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3484,7 +3484,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3555,7 +3555,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3626,7 +3626,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3697,7 +3697,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>['Germany', 'Netherlands']</t>
+          <t>['Netherlands', 'Germany']</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>['Bulgaria', 'Spain']</t>
+          <t>['Spain', 'Bulgaria']</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>['France', 'Spain']</t>
+          <t>['Spain', 'France']</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4182,7 +4182,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>['France', 'Spain']</t>
+          <t>['Spain', 'France']</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>['France', 'Spain']</t>
+          <t>['Spain', 'France']</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4312,7 +4312,7 @@
       <c r="I56" t="inlineStr"/>
       <c r="J56" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4379,7 +4379,7 @@
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4450,7 +4450,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4592,7 +4592,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -4805,7 +4805,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -4864,7 +4864,7 @@
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -4931,7 +4931,7 @@
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -4998,7 +4998,7 @@
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5917,7 +5917,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -6047,7 +6047,7 @@
       <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6114,7 +6114,7 @@
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -6189,7 +6189,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6536,7 +6536,7 @@
       <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -6603,7 +6603,7 @@
       <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -6820,7 +6820,7 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
@@ -6895,7 +6895,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
@@ -6966,7 +6966,7 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
@@ -7041,7 +7041,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -7116,7 +7116,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>['Portugal', 'England']</t>
+          <t>['England', 'Portugal']</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -7873,7 +7873,7 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
@@ -7940,7 +7940,7 @@
       <c r="I108" t="inlineStr"/>
       <c r="J108" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
@@ -8011,7 +8011,7 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K109" t="inlineStr">
@@ -8082,7 +8082,7 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
@@ -8153,7 +8153,7 @@
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
@@ -8224,7 +8224,7 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
@@ -8295,7 +8295,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K113" t="inlineStr">
@@ -8366,7 +8366,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
@@ -8437,7 +8437,7 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>['France', 'Netherlands']</t>
+          <t>['Netherlands', 'France']</t>
         </is>
       </c>
       <c r="K115" t="inlineStr">
@@ -8847,7 +8847,7 @@
       </c>
       <c r="J121" t="inlineStr">
         <is>
-          <t>['Portugal', 'Greece']</t>
+          <t>['Greece', 'Portugal']</t>
         </is>
       </c>
       <c r="K121" t="inlineStr">
@@ -10511,7 +10511,7 @@
       </c>
       <c r="J145" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K145" t="inlineStr">
@@ -10582,7 +10582,7 @@
       </c>
       <c r="J146" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K146" t="inlineStr">
@@ -10653,7 +10653,7 @@
       </c>
       <c r="J147" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K147" t="inlineStr">
@@ -10724,7 +10724,7 @@
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Netherlands']</t>
+          <t>['Netherlands', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K148" t="inlineStr">
@@ -11347,7 +11347,7 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey']</t>
+          <t>['Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K157" t="inlineStr">
@@ -11406,7 +11406,7 @@
       <c r="I158" t="inlineStr"/>
       <c r="J158" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K158" t="inlineStr">
@@ -11473,7 +11473,7 @@
       <c r="I159" t="inlineStr"/>
       <c r="J159" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K159" t="inlineStr">
@@ -11540,7 +11540,7 @@
       <c r="I160" t="inlineStr"/>
       <c r="J160" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K160" t="inlineStr">
@@ -11611,7 +11611,7 @@
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K161" t="inlineStr">
@@ -11682,7 +11682,7 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="K162" t="inlineStr">
@@ -11741,7 +11741,7 @@
       <c r="I163" t="inlineStr"/>
       <c r="J163" t="inlineStr">
         <is>
-          <t>['Romania', 'Netherlands']</t>
+          <t>['Netherlands', 'Romania']</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
@@ -11808,7 +11808,7 @@
       <c r="I164" t="inlineStr"/>
       <c r="J164" t="inlineStr">
         <is>
-          <t>['Romania', 'Netherlands']</t>
+          <t>['Netherlands', 'Romania']</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
@@ -11875,7 +11875,7 @@
       <c r="I165" t="inlineStr"/>
       <c r="J165" t="inlineStr">
         <is>
-          <t>['Romania', 'Netherlands']</t>
+          <t>['Netherlands', 'Romania']</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
@@ -11946,7 +11946,7 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>['Italy', 'Netherlands']</t>
+          <t>['Netherlands', 'Italy']</t>
         </is>
       </c>
       <c r="K166" t="inlineStr">
@@ -12017,7 +12017,7 @@
       </c>
       <c r="J167" t="inlineStr">
         <is>
-          <t>['Italy', 'Netherlands']</t>
+          <t>['Netherlands', 'Italy']</t>
         </is>
       </c>
       <c r="K167" t="inlineStr">
@@ -12088,7 +12088,7 @@
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>['Italy', 'Netherlands']</t>
+          <t>['Netherlands', 'Italy']</t>
         </is>
       </c>
       <c r="K168" t="inlineStr">
@@ -12159,7 +12159,7 @@
       </c>
       <c r="J169" t="inlineStr">
         <is>
-          <t>['Italy', 'Netherlands']</t>
+          <t>['Netherlands', 'Italy']</t>
         </is>
       </c>
       <c r="K169" t="inlineStr">
@@ -12218,7 +12218,7 @@
       <c r="I170" t="inlineStr"/>
       <c r="J170" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K170" t="inlineStr">
@@ -12285,7 +12285,7 @@
       <c r="I171" t="inlineStr"/>
       <c r="J171" t="inlineStr">
         <is>
-          <t>['Sweden', 'Spain']</t>
+          <t>['Spain', 'Sweden']</t>
         </is>
       </c>
       <c r="K171" t="inlineStr">
@@ -12356,7 +12356,7 @@
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="K172" t="inlineStr">
@@ -12427,7 +12427,7 @@
       </c>
       <c r="J173" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="K173" t="inlineStr">
@@ -12498,7 +12498,7 @@
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="K174" t="inlineStr">
@@ -12569,7 +12569,7 @@
       </c>
       <c r="J175" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="K175" t="inlineStr">
@@ -12640,7 +12640,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>['Spain', 'Russia']</t>
+          <t>['Russia', 'Spain']</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
@@ -12699,7 +12699,7 @@
       <c r="I177" t="inlineStr"/>
       <c r="J177" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -12766,7 +12766,7 @@
       <c r="I178" t="inlineStr"/>
       <c r="J178" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
@@ -12833,7 +12833,7 @@
       <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -12904,7 +12904,7 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Russia']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
@@ -12953,7 +12953,7 @@
         </is>
       </c>
       <c r="E181" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F181" t="n">
         <v>72</v>
@@ -12975,7 +12975,7 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>['Greece', 'Czech Republic']</t>
+          <t>['Russia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -12985,22 +12985,22 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
+          <t>Russia</t>
+        </is>
+      </c>
+      <c r="M181" t="inlineStr">
+        <is>
           <t>Greece</t>
         </is>
       </c>
-      <c r="M181" t="inlineStr">
-        <is>
-          <t>Russia</t>
-        </is>
-      </c>
       <c r="N181" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O181" t="n">
         <v>0</v>
       </c>
       <c r="P181" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="Q181" t="inlineStr"/>
     </row>
@@ -13105,7 +13105,7 @@
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>['Denmark', 'Germany']</t>
+          <t>['Germany', 'Denmark']</t>
         </is>
       </c>
       <c r="K183" t="inlineStr">
@@ -13176,7 +13176,7 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>['Denmark', 'Germany']</t>
+          <t>['Germany', 'Denmark']</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -13247,7 +13247,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>['Denmark', 'Germany']</t>
+          <t>['Germany', 'Denmark']</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
@@ -13296,7 +13296,7 @@
         </is>
       </c>
       <c r="E186" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F186" t="n">
         <v>28</v>
@@ -13318,7 +13318,7 @@
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>['Portugal', 'Germany']</t>
+          <t>['Germany', 'Denmark']</t>
         </is>
       </c>
       <c r="K186" t="inlineStr">
@@ -13328,16 +13328,16 @@
       </c>
       <c r="L186" t="inlineStr">
         <is>
+          <t>Denmark</t>
+        </is>
+      </c>
+      <c r="M186" t="inlineStr">
+        <is>
           <t>Portugal</t>
         </is>
       </c>
-      <c r="M186" t="inlineStr">
-        <is>
-          <t>Denmark</t>
-        </is>
-      </c>
       <c r="N186" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O186" t="n">
         <v>0</v>
@@ -13408,7 +13408,7 @@
         </is>
       </c>
       <c r="N187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O187" t="n">
         <v>2</v>
@@ -13523,7 +13523,7 @@
       <c r="I189" t="inlineStr"/>
       <c r="J189" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
@@ -13590,7 +13590,7 @@
       <c r="I190" t="inlineStr"/>
       <c r="J190" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
@@ -13657,7 +13657,7 @@
       <c r="I191" t="inlineStr"/>
       <c r="J191" t="inlineStr">
         <is>
-          <t>['Croatia', 'Spain']</t>
+          <t>['Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
@@ -13728,7 +13728,7 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>['Italy', 'Spain']</t>
+          <t>['Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
@@ -13799,7 +13799,7 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>['Italy', 'Spain']</t>
+          <t>['Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
@@ -13870,7 +13870,7 @@
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>['Italy', 'Spain']</t>
+          <t>['Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -14335,7 +14335,7 @@
       <c r="I201" t="inlineStr"/>
       <c r="J201" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France', 'Romania']</t>
+          <t>['Romania', 'Switzerland', 'France']</t>
         </is>
       </c>
       <c r="K201" t="inlineStr">
@@ -14402,7 +14402,7 @@
       <c r="I202" t="inlineStr"/>
       <c r="J202" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France', 'Romania']</t>
+          <t>['Romania', 'Switzerland', 'France']</t>
         </is>
       </c>
       <c r="K202" t="inlineStr">
@@ -14469,7 +14469,7 @@
       <c r="I203" t="inlineStr"/>
       <c r="J203" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France', 'Romania']</t>
+          <t>['Romania', 'Switzerland', 'France']</t>
         </is>
       </c>
       <c r="K203" t="inlineStr">
@@ -14599,7 +14599,7 @@
       <c r="I205" t="inlineStr"/>
       <c r="J205" t="inlineStr">
         <is>
-          <t>['England', 'Wales', 'Slovakia']</t>
+          <t>['Slovakia', 'England', 'Wales']</t>
         </is>
       </c>
       <c r="K205" t="inlineStr">
@@ -14666,7 +14666,7 @@
       <c r="I206" t="inlineStr"/>
       <c r="J206" t="inlineStr">
         <is>
-          <t>['England', 'Wales', 'Slovakia']</t>
+          <t>['Slovakia', 'England', 'Wales']</t>
         </is>
       </c>
       <c r="K206" t="inlineStr">
@@ -14737,7 +14737,7 @@
       <c r="I207" t="inlineStr"/>
       <c r="J207" t="inlineStr">
         <is>
-          <t>['England', 'Wales', 'Slovakia']</t>
+          <t>['Slovakia', 'England', 'Wales']</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
@@ -14812,7 +14812,7 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>['England', 'Wales', 'Slovakia']</t>
+          <t>['Slovakia', 'England', 'Wales']</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
@@ -14883,7 +14883,7 @@
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>['England', 'Wales', 'Slovakia']</t>
+          <t>['Slovakia', 'England', 'Wales']</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
@@ -14954,7 +14954,7 @@
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>['England', 'Wales', 'Slovakia']</t>
+          <t>['Slovakia', 'England', 'Wales']</t>
         </is>
       </c>
       <c r="K210" t="inlineStr">
@@ -15013,7 +15013,7 @@
       <c r="I211" t="inlineStr"/>
       <c r="J211" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Poland', 'Germany', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -15080,7 +15080,7 @@
       <c r="I212" t="inlineStr"/>
       <c r="J212" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Poland', 'Germany', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K212" t="inlineStr">
@@ -15147,7 +15147,7 @@
       <c r="I213" t="inlineStr"/>
       <c r="J213" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Poland', 'Germany', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K213" t="inlineStr">
@@ -15218,7 +15218,7 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Poland', 'Germany', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
@@ -15289,7 +15289,7 @@
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>['Poland', 'Northern Ireland', 'Germany']</t>
+          <t>['Poland', 'Germany', 'Northern Ireland']</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
@@ -15348,7 +15348,7 @@
       <c r="I216" t="inlineStr"/>
       <c r="J216" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'Spain']</t>
+          <t>['Spain', 'Czech Republic', 'Croatia']</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
@@ -15415,7 +15415,7 @@
       <c r="I217" t="inlineStr"/>
       <c r="J217" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'Spain']</t>
+          <t>['Spain', 'Czech Republic', 'Croatia']</t>
         </is>
       </c>
       <c r="K217" t="inlineStr">
@@ -15486,7 +15486,7 @@
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>['Croatia', 'Czech Republic', 'Spain']</t>
+          <t>['Spain', 'Czech Republic', 'Croatia']</t>
         </is>
       </c>
       <c r="K218" t="inlineStr">
@@ -15557,7 +15557,7 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>['Croatia', 'Turkey', 'Spain']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
@@ -15628,7 +15628,7 @@
       </c>
       <c r="J220" t="inlineStr">
         <is>
-          <t>['Croatia', 'Turkey', 'Spain']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K220" t="inlineStr">
@@ -15699,7 +15699,7 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>['Croatia', 'Turkey', 'Spain']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K221" t="inlineStr">
@@ -15770,7 +15770,7 @@
       </c>
       <c r="J222" t="inlineStr">
         <is>
-          <t>['Croatia', 'Turkey', 'Spain']</t>
+          <t>['Turkey', 'Spain', 'Croatia']</t>
         </is>
       </c>
       <c r="K222" t="inlineStr">
@@ -15829,7 +15829,7 @@
       <c r="I223" t="inlineStr"/>
       <c r="J223" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="K223" t="inlineStr">
@@ -15900,7 +15900,7 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="K224" t="inlineStr">
@@ -15971,7 +15971,7 @@
       </c>
       <c r="J225" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="K225" t="inlineStr">
@@ -16042,7 +16042,7 @@
       </c>
       <c r="J226" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="K226" t="inlineStr">
@@ -16113,7 +16113,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
@@ -16184,7 +16184,7 @@
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
@@ -16255,7 +16255,7 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
@@ -16326,7 +16326,7 @@
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
@@ -16397,7 +16397,7 @@
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
@@ -16468,7 +16468,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>['Portugal', 'Iceland', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'Iceland']</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
@@ -16527,7 +16527,7 @@
       <c r="I233" t="inlineStr"/>
       <c r="J233" t="inlineStr">
         <is>
-          <t>['Italy', 'Sweden', 'Belgium']</t>
+          <t>['Sweden', 'Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
@@ -16594,7 +16594,7 @@
       <c r="I234" t="inlineStr"/>
       <c r="J234" t="inlineStr">
         <is>
-          <t>['Italy', 'Sweden', 'Belgium']</t>
+          <t>['Sweden', 'Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
@@ -16661,7 +16661,7 @@
       <c r="I235" t="inlineStr"/>
       <c r="J235" t="inlineStr">
         <is>
-          <t>['Italy', 'Sweden', 'Belgium']</t>
+          <t>['Sweden', 'Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
@@ -16732,7 +16732,7 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>['Italy', 'Republic of Ireland', 'Belgium']</t>
+          <t>['Republic of Ireland', 'Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
@@ -16803,7 +16803,7 @@
       </c>
       <c r="J237" t="inlineStr">
         <is>
-          <t>['Italy', 'Republic of Ireland', 'Belgium']</t>
+          <t>['Republic of Ireland', 'Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="K237" t="inlineStr">
@@ -16874,7 +16874,7 @@
       </c>
       <c r="J238" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Wales', 'Switzerland', 'Italy']</t>
         </is>
       </c>
       <c r="K238" t="inlineStr">
@@ -16945,7 +16945,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Wales', 'Switzerland', 'Italy']</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
@@ -17016,7 +17016,7 @@
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Wales', 'Switzerland', 'Italy']</t>
         </is>
       </c>
       <c r="K240" t="inlineStr">
@@ -17087,7 +17087,7 @@
       </c>
       <c r="J241" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Wales', 'Switzerland', 'Italy']</t>
         </is>
       </c>
       <c r="K241" t="inlineStr">
@@ -17146,7 +17146,7 @@
       <c r="I242" t="inlineStr"/>
       <c r="J242" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Wales', 'Switzerland', 'Italy']</t>
         </is>
       </c>
       <c r="K242" t="inlineStr">
@@ -17213,7 +17213,7 @@
       <c r="I243" t="inlineStr"/>
       <c r="J243" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Wales', 'Switzerland', 'Italy']</t>
         </is>
       </c>
       <c r="K243" t="inlineStr">
@@ -17284,7 +17284,7 @@
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Italy', 'Wales']</t>
+          <t>['Wales', 'Switzerland', 'Italy']</t>
         </is>
       </c>
       <c r="K244" t="inlineStr">
@@ -17343,7 +17343,7 @@
       <c r="I245" t="inlineStr"/>
       <c r="J245" t="inlineStr">
         <is>
-          <t>['Austria', 'Ukraine', 'Netherlands']</t>
+          <t>['Netherlands', 'Ukraine', 'Austria']</t>
         </is>
       </c>
       <c r="K245" t="inlineStr">
@@ -17410,7 +17410,7 @@
       <c r="I246" t="inlineStr"/>
       <c r="J246" t="inlineStr">
         <is>
-          <t>['Austria', 'Ukraine', 'Netherlands']</t>
+          <t>['Netherlands', 'Ukraine', 'Austria']</t>
         </is>
       </c>
       <c r="K246" t="inlineStr">
@@ -17481,7 +17481,7 @@
       </c>
       <c r="J247" t="inlineStr">
         <is>
-          <t>['Austria', 'Ukraine', 'Netherlands']</t>
+          <t>['Netherlands', 'Ukraine', 'Austria']</t>
         </is>
       </c>
       <c r="K247" t="inlineStr">
@@ -17548,7 +17548,7 @@
       <c r="I248" t="inlineStr"/>
       <c r="J248" t="inlineStr">
         <is>
-          <t>['Austria', 'Ukraine', 'Netherlands']</t>
+          <t>['Netherlands', 'Ukraine', 'Austria']</t>
         </is>
       </c>
       <c r="K248" t="inlineStr">
@@ -17619,7 +17619,7 @@
       </c>
       <c r="J249" t="inlineStr">
         <is>
-          <t>['Austria', 'Ukraine', 'Netherlands']</t>
+          <t>['Netherlands', 'Ukraine', 'Austria']</t>
         </is>
       </c>
       <c r="K249" t="inlineStr">
@@ -17690,7 +17690,7 @@
       </c>
       <c r="J250" t="inlineStr">
         <is>
-          <t>['Austria', 'Ukraine', 'Netherlands']</t>
+          <t>['Netherlands', 'Ukraine', 'Austria']</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
@@ -17761,7 +17761,7 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>['Austria', 'Ukraine', 'Netherlands']</t>
+          <t>['Netherlands', 'Ukraine', 'Austria']</t>
         </is>
       </c>
       <c r="K251" t="inlineStr">
@@ -17958,7 +17958,7 @@
       </c>
       <c r="J254" t="inlineStr">
         <is>
-          <t>['Denmark', 'Russia', 'Belgium']</t>
+          <t>['Russia', 'Denmark', 'Belgium']</t>
         </is>
       </c>
       <c r="K254" t="inlineStr">
@@ -18029,7 +18029,7 @@
       </c>
       <c r="J255" t="inlineStr">
         <is>
-          <t>['Denmark', 'Russia', 'Belgium']</t>
+          <t>['Russia', 'Denmark', 'Belgium']</t>
         </is>
       </c>
       <c r="K255" t="inlineStr">
@@ -18313,7 +18313,7 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>['Denmark', 'Russia', 'Belgium']</t>
+          <t>['Russia', 'Denmark', 'Belgium']</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
@@ -18384,7 +18384,7 @@
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>['Denmark', 'Russia', 'Belgium']</t>
+          <t>['Russia', 'Denmark', 'Belgium']</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
@@ -18443,7 +18443,7 @@
       <c r="I261" t="inlineStr"/>
       <c r="J261" t="inlineStr">
         <is>
-          <t>['Croatia', 'England', 'Czech Republic']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K261" t="inlineStr">
@@ -18510,7 +18510,7 @@
       <c r="I262" t="inlineStr"/>
       <c r="J262" t="inlineStr">
         <is>
-          <t>['Croatia', 'England', 'Czech Republic']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
@@ -18581,7 +18581,7 @@
       </c>
       <c r="J263" t="inlineStr">
         <is>
-          <t>['Croatia', 'England', 'Czech Republic']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
@@ -18652,7 +18652,7 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>['Croatia', 'England', 'Czech Republic']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
@@ -18723,7 +18723,7 @@
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>['Croatia', 'England', 'Czech Republic']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K265" t="inlineStr">
@@ -18794,7 +18794,7 @@
       </c>
       <c r="J266" t="inlineStr">
         <is>
-          <t>['Croatia', 'England', 'Czech Republic']</t>
+          <t>['England', 'Croatia', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K266" t="inlineStr">
@@ -18865,7 +18865,7 @@
       </c>
       <c r="J267" t="inlineStr">
         <is>
-          <t>['Croatia', 'England', 'Czech Republic']</t>
+          <t>['England', 'Czech Republic', 'Croatia']</t>
         </is>
       </c>
       <c r="K267" t="inlineStr">
@@ -18936,7 +18936,7 @@
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K268" t="inlineStr">
@@ -19007,7 +19007,7 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K269" t="inlineStr">
@@ -19078,7 +19078,7 @@
       </c>
       <c r="J270" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K270" t="inlineStr">
@@ -19149,7 +19149,7 @@
       </c>
       <c r="J271" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K271" t="inlineStr">
@@ -19220,7 +19220,7 @@
       </c>
       <c r="J272" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K272" t="inlineStr">
@@ -19279,7 +19279,7 @@
       <c r="I273" t="inlineStr"/>
       <c r="J273" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K273" t="inlineStr">
@@ -19346,7 +19346,7 @@
       <c r="I274" t="inlineStr"/>
       <c r="J274" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K274" t="inlineStr">
@@ -19417,7 +19417,7 @@
       </c>
       <c r="J275" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K275" t="inlineStr">
@@ -19488,7 +19488,7 @@
       </c>
       <c r="J276" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K276" t="inlineStr">
@@ -19559,7 +19559,7 @@
       </c>
       <c r="J277" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K277" t="inlineStr">
@@ -19630,7 +19630,7 @@
       </c>
       <c r="J278" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K278" t="inlineStr">
@@ -19701,7 +19701,7 @@
       </c>
       <c r="J279" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden', 'Spain']</t>
+          <t>['Spain', 'Slovakia', 'Sweden']</t>
         </is>
       </c>
       <c r="K279" t="inlineStr">
@@ -19760,7 +19760,7 @@
       <c r="I280" t="inlineStr"/>
       <c r="J280" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Germany']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K280" t="inlineStr">
@@ -19831,7 +19831,7 @@
       </c>
       <c r="J281" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K281" t="inlineStr">
@@ -19902,7 +19902,7 @@
       </c>
       <c r="J282" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K282" t="inlineStr">
@@ -19973,7 +19973,7 @@
       </c>
       <c r="J283" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K283" t="inlineStr">
@@ -20044,7 +20044,7 @@
       </c>
       <c r="J284" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K284" t="inlineStr">
@@ -20115,7 +20115,7 @@
       </c>
       <c r="J285" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Germany']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K285" t="inlineStr">
@@ -20186,7 +20186,7 @@
       </c>
       <c r="J286" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Hungary']</t>
+          <t>['Portugal', 'Hungary', 'France']</t>
         </is>
       </c>
       <c r="K286" t="inlineStr">
@@ -20257,7 +20257,7 @@
       </c>
       <c r="J287" t="inlineStr">
         <is>
-          <t>['Portugal', 'France', 'Germany']</t>
+          <t>['Portugal', 'Germany', 'France']</t>
         </is>
       </c>
       <c r="K287" t="inlineStr">
@@ -20316,7 +20316,7 @@
       <c r="I288" t="inlineStr"/>
       <c r="J288" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Scotland', 'Germany']</t>
+          <t>['Germany', 'Switzerland', 'Scotland']</t>
         </is>
       </c>
       <c r="K288" t="inlineStr">
@@ -20383,7 +20383,7 @@
       <c r="I289" t="inlineStr"/>
       <c r="J289" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Scotland', 'Germany']</t>
+          <t>['Germany', 'Switzerland', 'Scotland']</t>
         </is>
       </c>
       <c r="K289" t="inlineStr">
@@ -20454,7 +20454,7 @@
       </c>
       <c r="J290" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Scotland', 'Germany']</t>
+          <t>['Germany', 'Switzerland', 'Scotland']</t>
         </is>
       </c>
       <c r="K290" t="inlineStr">
@@ -20525,7 +20525,7 @@
       </c>
       <c r="J291" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Scotland', 'Germany']</t>
+          <t>['Germany', 'Switzerland', 'Scotland']</t>
         </is>
       </c>
       <c r="K291" t="inlineStr">
@@ -20596,7 +20596,7 @@
       </c>
       <c r="J292" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Hungary', 'Germany']</t>
+          <t>['Hungary', 'Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="K292" t="inlineStr">
@@ -20655,7 +20655,7 @@
       <c r="I293" t="inlineStr"/>
       <c r="J293" t="inlineStr">
         <is>
-          <t>['Albania', 'Italy', 'Spain']</t>
+          <t>['Albania', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K293" t="inlineStr">
@@ -20722,7 +20722,7 @@
       <c r="I294" t="inlineStr"/>
       <c r="J294" t="inlineStr">
         <is>
-          <t>['Albania', 'Italy', 'Spain']</t>
+          <t>['Albania', 'Spain', 'Italy']</t>
         </is>
       </c>
       <c r="K294" t="inlineStr">
@@ -20793,7 +20793,7 @@
       </c>
       <c r="J295" t="inlineStr">
         <is>
-          <t>['Croatia', 'Italy', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Italy']</t>
         </is>
       </c>
       <c r="K295" t="inlineStr">
@@ -20864,7 +20864,7 @@
       </c>
       <c r="J296" t="inlineStr">
         <is>
-          <t>['Croatia', 'Italy', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Italy']</t>
         </is>
       </c>
       <c r="K296" t="inlineStr">
@@ -20935,7 +20935,7 @@
       </c>
       <c r="J297" t="inlineStr">
         <is>
-          <t>['Croatia', 'Italy', 'Spain']</t>
+          <t>['Spain', 'Croatia', 'Italy']</t>
         </is>
       </c>
       <c r="K297" t="inlineStr">
@@ -20994,7 +20994,7 @@
       <c r="I298" t="inlineStr"/>
       <c r="J298" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K298" t="inlineStr">
@@ -21065,7 +21065,7 @@
       </c>
       <c r="J299" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K299" t="inlineStr">
@@ -21136,7 +21136,7 @@
       </c>
       <c r="J300" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K300" t="inlineStr">
@@ -21207,7 +21207,7 @@
       </c>
       <c r="J301" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K301" t="inlineStr">
@@ -21278,7 +21278,7 @@
       </c>
       <c r="J302" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K302" t="inlineStr">
@@ -21349,7 +21349,7 @@
       </c>
       <c r="J303" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K303" t="inlineStr">
@@ -21420,7 +21420,7 @@
       </c>
       <c r="J304" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K304" t="inlineStr">
@@ -21491,7 +21491,7 @@
       </c>
       <c r="J305" t="inlineStr">
         <is>
-          <t>['France', 'Austria', 'Netherlands']</t>
+          <t>['Netherlands', 'France', 'Austria']</t>
         </is>
       </c>
       <c r="K305" t="inlineStr">
@@ -21550,7 +21550,7 @@
       <c r="I306" t="inlineStr"/>
       <c r="J306" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England', 'Denmark']</t>
+          <t>['England', 'Slovenia', 'Denmark']</t>
         </is>
       </c>
       <c r="K306" t="inlineStr">
@@ -21617,7 +21617,7 @@
       <c r="I307" t="inlineStr"/>
       <c r="J307" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England', 'Denmark']</t>
+          <t>['England', 'Slovenia', 'Denmark']</t>
         </is>
       </c>
       <c r="K307" t="inlineStr">
@@ -21684,7 +21684,7 @@
       <c r="I308" t="inlineStr"/>
       <c r="J308" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England', 'Denmark']</t>
+          <t>['England', 'Slovenia', 'Denmark']</t>
         </is>
       </c>
       <c r="K308" t="inlineStr">
@@ -21743,7 +21743,7 @@
       <c r="I309" t="inlineStr"/>
       <c r="J309" t="inlineStr">
         <is>
-          <t>['Ukraine', 'Romania', 'Belgium']</t>
+          <t>['Romania', 'Ukraine', 'Belgium']</t>
         </is>
       </c>
       <c r="K309" t="inlineStr">
@@ -21810,7 +21810,7 @@
       <c r="I310" t="inlineStr"/>
       <c r="J310" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Romania', 'Belgium']</t>
+          <t>['Romania', 'Slovakia', 'Belgium']</t>
         </is>
       </c>
       <c r="K310" t="inlineStr">
@@ -21881,7 +21881,7 @@
       </c>
       <c r="J311" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Ukraine', 'Belgium']</t>
+          <t>['Ukraine', 'Slovakia', 'Belgium']</t>
         </is>
       </c>
       <c r="K311" t="inlineStr">
@@ -21952,7 +21952,7 @@
       </c>
       <c r="J312" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Romania', 'Belgium']</t>
+          <t>['Romania', 'Slovakia', 'Belgium']</t>
         </is>
       </c>
       <c r="K312" t="inlineStr">
@@ -22011,7 +22011,7 @@
       <c r="I313" t="inlineStr"/>
       <c r="J313" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Czech Republic']</t>
+          <t>['Turkey', 'Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K313" t="inlineStr">
@@ -22078,7 +22078,7 @@
       <c r="I314" t="inlineStr"/>
       <c r="J314" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Czech Republic']</t>
+          <t>['Turkey', 'Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="K314" t="inlineStr">
@@ -22149,7 +22149,7 @@
       </c>
       <c r="J315" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Georgia', 'Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K315" t="inlineStr">
@@ -22224,7 +22224,7 @@
       </c>
       <c r="J316" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Georgia', 'Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K316" t="inlineStr">
@@ -22295,7 +22295,7 @@
       </c>
       <c r="J317" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Georgia', 'Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K317" t="inlineStr">
@@ -22366,7 +22366,7 @@
       </c>
       <c r="J318" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Georgia', 'Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K318" t="inlineStr">
@@ -22441,7 +22441,7 @@
       </c>
       <c r="J319" t="inlineStr">
         <is>
-          <t>['Portugal', 'Turkey', 'Georgia']</t>
+          <t>['Georgia', 'Turkey', 'Portugal']</t>
         </is>
       </c>
       <c r="K319" t="inlineStr">

</xml_diff>